<commit_message>
Added initial simulation data
</commit_message>
<xml_diff>
--- a/simulations_metadata.xlsx
+++ b/simulations_metadata.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="36">
   <si>
     <t>NS to S</t>
   </si>
@@ -120,6 +120,21 @@
   </si>
   <si>
     <t>param01seed0.25</t>
+  </si>
+  <si>
+    <t>param01seed0.30</t>
+  </si>
+  <si>
+    <t>param01seed0.35</t>
+  </si>
+  <si>
+    <t>param01seed0.40</t>
+  </si>
+  <si>
+    <t>param01seed0.45</t>
+  </si>
+  <si>
+    <t>param01seed0.50</t>
   </si>
 </sst>
 </file>
@@ -457,7 +472,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -736,7 +751,7 @@
         <v>28</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
@@ -790,7 +805,7 @@
         <v>29</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
@@ -844,6 +859,276 @@
         <v>30</v>
       </c>
       <c r="Q7" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E8" s="4">
+        <f>0.3*(F8+G8+H8+I8)</f>
+        <v>0.16874999999999998</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="H8" s="2">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E9" s="4">
+        <f>0.35*(F9+G9+H9+I9)</f>
+        <v>0.19687499999999999</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="H9" s="2">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E10" s="4">
+        <f>0.4*(F10+G10+H10+I10)</f>
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="H10" s="2">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E11" s="4">
+        <f>0.45*(F11+G11+H11+I11)</f>
+        <v>0.25312499999999999</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="H11" s="2">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E12" s="4">
+        <f>0.5*(F12+G12+H12+I12)</f>
+        <v>0.28125</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="H12" s="2">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q12" s="2" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added param04 data and updated progress
</commit_message>
<xml_diff>
--- a/simulations_metadata.xlsx
+++ b/simulations_metadata.xlsx
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="69">
   <si>
     <t>NS to S</t>
   </si>
@@ -150,9 +150,6 @@
     <t>param01seed0.05</t>
   </si>
   <si>
-    <t>RUNNING</t>
-  </si>
-  <si>
     <t>seed params</t>
   </si>
   <si>
@@ -238,6 +235,54 @@
   </si>
   <si>
     <t>param04seed0.15</t>
+  </si>
+  <si>
+    <t>param04seed0.01</t>
+  </si>
+  <si>
+    <t>param04seed0.20</t>
+  </si>
+  <si>
+    <t>param04seed0.25</t>
+  </si>
+  <si>
+    <t>param04seed0.30</t>
+  </si>
+  <si>
+    <t>param04seed0.35</t>
+  </si>
+  <si>
+    <t>param04seed0.40</t>
+  </si>
+  <si>
+    <t>param04seed0.45</t>
+  </si>
+  <si>
+    <t>param05seed0.00</t>
+  </si>
+  <si>
+    <t>param05seed0.05</t>
+  </si>
+  <si>
+    <t>param05seed0.01</t>
+  </si>
+  <si>
+    <t>GQ  (qsub)</t>
+  </si>
+  <si>
+    <t>param05seed0.10</t>
+  </si>
+  <si>
+    <t>param05seed0.15</t>
+  </si>
+  <si>
+    <t>param05seed0.20</t>
+  </si>
+  <si>
+    <t>param05seed0.25</t>
+  </si>
+  <si>
+    <t>NOT QSUB'D YET (waiting for queue)</t>
   </si>
 </sst>
 </file>
@@ -628,7 +673,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q30"/>
+  <dimension ref="A1:Q45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -641,7 +686,8 @@
     <col min="5" max="5" width="11.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="15" width="10.83203125" style="2"/>
     <col min="16" max="16" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="10.83203125" style="2"/>
+    <col min="17" max="17" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -652,7 +698,7 @@
         <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -694,7 +740,7 @@
         <v>20</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -705,7 +751,7 @@
         <v>16</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" s="5">
         <v>999999</v>
@@ -748,7 +794,7 @@
         <v>21</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -759,7 +805,7 @@
         <v>16</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" s="5">
         <v>999999</v>
@@ -802,7 +848,7 @@
         <v>23</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
@@ -813,7 +859,7 @@
         <v>16</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="5">
         <v>999999</v>
@@ -856,7 +902,7 @@
         <v>22</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
@@ -867,7 +913,7 @@
         <v>16</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" s="5">
         <v>999999</v>
@@ -907,10 +953,10 @@
         <v>12</v>
       </c>
       <c r="P5" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q5" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
@@ -921,7 +967,7 @@
         <v>16</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" s="5">
         <v>999999</v>
@@ -961,10 +1007,10 @@
         <v>12</v>
       </c>
       <c r="P6" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q6" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
@@ -975,7 +1021,7 @@
         <v>16</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" s="5">
         <v>999999</v>
@@ -1015,10 +1061,10 @@
         <v>12</v>
       </c>
       <c r="P7" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q7" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
@@ -1029,7 +1075,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" s="5">
         <v>999999</v>
@@ -1069,10 +1115,10 @@
         <v>12</v>
       </c>
       <c r="P8" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
@@ -1083,7 +1129,7 @@
         <v>16</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" s="5">
         <v>999999</v>
@@ -1123,10 +1169,10 @@
         <v>12</v>
       </c>
       <c r="P9" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q9" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
@@ -1137,7 +1183,7 @@
         <v>16</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" s="5">
         <v>999999</v>
@@ -1177,10 +1223,10 @@
         <v>12</v>
       </c>
       <c r="P10" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Q10" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
@@ -1191,7 +1237,7 @@
         <v>16</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D11" s="5">
         <v>999999</v>
@@ -1231,10 +1277,10 @@
         <v>12</v>
       </c>
       <c r="P11" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q11" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
@@ -1245,7 +1291,7 @@
         <v>16</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" s="5">
         <v>999999</v>
@@ -1285,10 +1331,10 @@
         <v>12</v>
       </c>
       <c r="P12" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q12" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
@@ -1299,7 +1345,7 @@
         <v>16</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D14" s="7">
         <v>999999</v>
@@ -1339,10 +1385,10 @@
         <v>12</v>
       </c>
       <c r="P14" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q14" s="7" t="s">
         <v>37</v>
-      </c>
-      <c r="Q14" s="7" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
@@ -1353,7 +1399,7 @@
         <v>16</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D15" s="7">
         <v>999999</v>
@@ -1393,10 +1439,10 @@
         <v>12</v>
       </c>
       <c r="P15" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q15" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
@@ -1407,7 +1453,7 @@
         <v>16</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D16" s="7">
         <v>999999</v>
@@ -1447,10 +1493,10 @@
         <v>12</v>
       </c>
       <c r="P16" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q16" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
@@ -1461,7 +1507,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D17" s="7">
         <v>999999</v>
@@ -1501,10 +1547,10 @@
         <v>12</v>
       </c>
       <c r="P17" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q17" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
@@ -1515,7 +1561,7 @@
         <v>16</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D19" s="5">
         <v>999999</v>
@@ -1555,10 +1601,10 @@
         <v>12</v>
       </c>
       <c r="P19" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Q19" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
@@ -1569,7 +1615,7 @@
         <v>16</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D20" s="5">
         <v>999999</v>
@@ -1609,10 +1655,10 @@
         <v>12</v>
       </c>
       <c r="P20" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q20" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
@@ -1623,7 +1669,7 @@
         <v>16</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D21" s="5">
         <v>999999</v>
@@ -1663,10 +1709,10 @@
         <v>12</v>
       </c>
       <c r="P21" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q21" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
@@ -1677,7 +1723,7 @@
         <v>16</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D22" s="5">
         <v>999999</v>
@@ -1717,10 +1763,10 @@
         <v>12</v>
       </c>
       <c r="P22" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q22" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
@@ -1731,7 +1777,7 @@
         <v>16</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D23" s="5">
         <v>999999</v>
@@ -1771,10 +1817,10 @@
         <v>12</v>
       </c>
       <c r="P23" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Q23" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
@@ -1785,7 +1831,7 @@
         <v>16</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D24" s="5">
         <v>999999</v>
@@ -1825,10 +1871,10 @@
         <v>12</v>
       </c>
       <c r="P24" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q24" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
@@ -1839,7 +1885,7 @@
         <v>16</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D25" s="5">
         <v>999999</v>
@@ -1879,10 +1925,10 @@
         <v>12</v>
       </c>
       <c r="P25" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Q25" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
@@ -1893,7 +1939,7 @@
         <v>16</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D27" s="2">
         <v>999999</v>
@@ -1933,10 +1979,10 @@
         <v>12</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q27" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
@@ -1947,50 +1993,50 @@
         <v>16</v>
       </c>
       <c r="C28" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E28" s="4">
+        <f>0.01*G28</f>
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="F28" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="G28" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="H28" s="2">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="I28" s="2">
+        <v>0</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P28" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q28" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="D28" s="2">
-        <v>999999</v>
-      </c>
-      <c r="E28" s="4">
-        <f>0.05*G28</f>
-        <v>4.4999999999999997E-3</v>
-      </c>
-      <c r="F28" s="2">
-        <v>0.45</v>
-      </c>
-      <c r="G28" s="2">
-        <v>0.09</v>
-      </c>
-      <c r="H28" s="2">
-        <v>2.2499999999999999E-2</v>
-      </c>
-      <c r="I28" s="2">
-        <v>0</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K28" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L28" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="M28" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="N28" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O28" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="P28" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q28" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
@@ -2001,50 +2047,50 @@
         <v>16</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E29" s="4">
+        <f>0.05*G29</f>
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="F29" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="G29" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="H29" s="2">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="I29" s="2">
+        <v>0</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P29" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q29" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="D29" s="2">
-        <v>999999</v>
-      </c>
-      <c r="E29" s="4">
-        <f>0.1*G29</f>
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="F29" s="2">
-        <v>0.45</v>
-      </c>
-      <c r="G29" s="2">
-        <v>0.09</v>
-      </c>
-      <c r="H29" s="2">
-        <v>2.2499999999999999E-2</v>
-      </c>
-      <c r="I29" s="2">
-        <v>0</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K29" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L29" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="M29" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="N29" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O29" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="P29" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q29" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
@@ -2055,50 +2101,806 @@
         <v>16</v>
       </c>
       <c r="C30" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E30" s="4">
+        <f>0.1*G30</f>
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="F30" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="G30" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="H30" s="2">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="I30" s="2">
+        <v>0</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P30" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q30" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D30" s="2">
-        <v>999999</v>
-      </c>
-      <c r="E30" s="4">
-        <f>0.15*G30</f>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E31" s="4">
+        <f>0.15*G31</f>
         <v>1.35E-2</v>
       </c>
-      <c r="F30" s="2">
-        <v>0.45</v>
-      </c>
-      <c r="G30" s="2">
-        <v>0.09</v>
-      </c>
-      <c r="H30" s="2">
-        <v>2.2499999999999999E-2</v>
-      </c>
-      <c r="I30" s="2">
-        <v>0</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K30" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L30" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="M30" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="N30" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O30" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="P30" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q30" s="2" t="s">
-        <v>24</v>
+      <c r="F31" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="G31" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="H31" s="2">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="I31" s="2">
+        <v>0</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P31" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q31" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E32" s="4">
+        <f>0.2*G32</f>
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="F32" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="G32" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="H32" s="2">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="I32" s="2">
+        <v>0</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P32" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q32" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D33" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E33" s="4">
+        <f>0.25*G33</f>
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="F33" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="G33" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="H33" s="2">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="I33" s="2">
+        <v>0</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M33" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P33" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q33" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D34" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E34" s="4">
+        <f>0.3*G34</f>
+        <v>2.7E-2</v>
+      </c>
+      <c r="F34" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="G34" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="H34" s="2">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="I34" s="2">
+        <v>0</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P34" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q34" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D35" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E35" s="4">
+        <f>0.35*G35</f>
+        <v>3.15E-2</v>
+      </c>
+      <c r="F35" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="G35" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="H35" s="2">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="I35" s="2">
+        <v>0</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P35" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q35" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D36" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E36" s="4">
+        <f>0.4*G36</f>
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="F36" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="G36" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="H36" s="2">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="I36" s="2">
+        <v>0</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L36" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M36" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P36" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q36" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E37" s="4">
+        <f>0.45*G37</f>
+        <v>4.0500000000000001E-2</v>
+      </c>
+      <c r="F37" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="G37" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="H37" s="2">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="I37" s="2">
+        <v>0</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L37" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M37" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N37" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O37" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P37" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q37" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D39" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E39" s="4">
+        <f>0*G39</f>
+        <v>0</v>
+      </c>
+      <c r="F39" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="G39" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="H39" s="2">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="I39" s="2">
+        <v>0</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L39" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M39" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N39" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O39" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P39" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q39" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D40" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E40" s="4">
+        <f>0.01*G40</f>
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="F40" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="G40" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="H40" s="2">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="I40" s="2">
+        <v>0</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L40" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M40" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N40" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O40" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P40" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q40" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D41" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E41" s="4">
+        <f>0.05*G41</f>
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="F41" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="G41" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="H41" s="2">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="I41" s="2">
+        <v>0</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L41" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M41" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N41" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O41" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P41" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q41" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D42" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E42" s="4">
+        <f>0.1*G42</f>
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="F42" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="G42" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="H42" s="2">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="I42" s="2">
+        <v>0</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K42" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L42" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M42" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N42" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O42" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P42" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q42" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D43" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E43" s="4">
+        <f>0.15*G43</f>
+        <v>1.35E-2</v>
+      </c>
+      <c r="F43" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="G43" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="H43" s="2">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="I43" s="2">
+        <v>0</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L43" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M43" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N43" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O43" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P43" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q43" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D44" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E44" s="4">
+        <f>0.2*G44</f>
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="F44" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="G44" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="H44" s="2">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="I44" s="2">
+        <v>0</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L44" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M44" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N44" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O44" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P44" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q44" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D45" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E45" s="4">
+        <f>0.25*G45</f>
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="F45" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="G45" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="H45" s="2">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="I45" s="2">
+        <v>0</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L45" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M45" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N45" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O45" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P45" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q45" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added data and updated metadata
</commit_message>
<xml_diff>
--- a/simulations_metadata.xlsx
+++ b/simulations_metadata.xlsx
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="84">
   <si>
     <t>NS to S</t>
   </si>
@@ -267,9 +267,6 @@
     <t>param05seed0.01</t>
   </si>
   <si>
-    <t>GQ  (qsub)</t>
-  </si>
-  <si>
     <t>param05seed0.10</t>
   </si>
   <si>
@@ -282,7 +279,55 @@
     <t>param05seed0.25</t>
   </si>
   <si>
-    <t>NOT QSUB'D YET (waiting for queue)</t>
+    <t>param05seed0.30</t>
+  </si>
+  <si>
+    <t>param05seed0.35</t>
+  </si>
+  <si>
+    <t>param05seed0.40</t>
+  </si>
+  <si>
+    <t>param05seed0.45</t>
+  </si>
+  <si>
+    <t>param06seed0.00</t>
+  </si>
+  <si>
+    <t>365/365</t>
+  </si>
+  <si>
+    <t>param06seed0.01</t>
+  </si>
+  <si>
+    <t>GQ (qsub)</t>
+  </si>
+  <si>
+    <t>param06seed0.05</t>
+  </si>
+  <si>
+    <t>param06seed0.10</t>
+  </si>
+  <si>
+    <t>param06seed0.15</t>
+  </si>
+  <si>
+    <t>param06seed0.20</t>
+  </si>
+  <si>
+    <t>param06seed0.25</t>
+  </si>
+  <si>
+    <t>param06seed0.30</t>
+  </si>
+  <si>
+    <t>param06seed0.35</t>
+  </si>
+  <si>
+    <t>param06seed0.40</t>
+  </si>
+  <si>
+    <t>param06seed0.45</t>
   </si>
 </sst>
 </file>
@@ -360,8 +405,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -395,9 +442,11 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -673,7 +722,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q45"/>
+  <dimension ref="A1:Q61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2630,7 +2679,7 @@
         <v>62</v>
       </c>
       <c r="Q40" s="2" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.2">
@@ -2684,7 +2733,7 @@
         <v>61</v>
       </c>
       <c r="Q41" s="2" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.2">
@@ -2735,10 +2784,10 @@
         <v>12</v>
       </c>
       <c r="P42" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q42" s="2" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.2">
@@ -2789,10 +2838,10 @@
         <v>12</v>
       </c>
       <c r="P43" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Q43" s="2" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.2">
@@ -2843,10 +2892,10 @@
         <v>12</v>
       </c>
       <c r="P44" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q44" s="2" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.2">
@@ -2897,10 +2946,820 @@
         <v>12</v>
       </c>
       <c r="P45" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q45" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D46" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E46" s="4">
+        <f>0.3*G46</f>
+        <v>2.7E-2</v>
+      </c>
+      <c r="F46" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="G46" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="H46" s="2">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="I46" s="2">
+        <v>0</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L46" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M46" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N46" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O46" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P46" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="Q45" s="2" t="s">
+      <c r="Q46" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D47" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E47" s="4">
+        <f>0.35*G47</f>
+        <v>3.15E-2</v>
+      </c>
+      <c r="F47" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="G47" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="H47" s="2">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="I47" s="2">
+        <v>0</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L47" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M47" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N47" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O47" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P47" s="2" t="s">
         <v>68</v>
+      </c>
+      <c r="Q47" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D48" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E48" s="4">
+        <f>0.4*G48</f>
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="F48" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="G48" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="H48" s="2">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="I48" s="2">
+        <v>0</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K48" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L48" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M48" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N48" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O48" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P48" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q48" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D49" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E49" s="4">
+        <f>0.45*G49</f>
+        <v>4.0500000000000001E-2</v>
+      </c>
+      <c r="F49" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="G49" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="H49" s="2">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="I49" s="2">
+        <v>0</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L49" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M49" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N49" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O49" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P49" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q49" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D51" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E51" s="4">
+        <f>0*G51</f>
+        <v>0</v>
+      </c>
+      <c r="F51" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="G51" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="H51" s="2">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="I51" s="2">
+        <v>0</v>
+      </c>
+      <c r="J51" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K51" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L51" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="M51" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N51" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O51" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P51" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q51" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D52" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E52" s="4">
+        <f>0.01*G52</f>
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="F52" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="G52" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="H52" s="2">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="I52" s="2">
+        <v>0</v>
+      </c>
+      <c r="J52" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K52" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L52" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="M52" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N52" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O52" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P52" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q52" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D53" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E53" s="4">
+        <f>0.05*G53</f>
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="F53" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="G53" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="H53" s="2">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="I53" s="2">
+        <v>0</v>
+      </c>
+      <c r="J53" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K53" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L53" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="M53" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N53" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O53" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P53" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q53" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D54" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E54" s="4">
+        <f>0.1*G54</f>
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="F54" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="G54" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="H54" s="2">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="I54" s="2">
+        <v>0</v>
+      </c>
+      <c r="J54" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K54" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L54" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="M54" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N54" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O54" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P54" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q54" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D55" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E55" s="4">
+        <f>0.15*G55</f>
+        <v>1.35E-2</v>
+      </c>
+      <c r="F55" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="G55" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="H55" s="2">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="I55" s="2">
+        <v>0</v>
+      </c>
+      <c r="J55" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K55" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L55" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="M55" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N55" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O55" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P55" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q55" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D56" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E56" s="4">
+        <f>0.2*G56</f>
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="F56" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="G56" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="H56" s="2">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="I56" s="2">
+        <v>0</v>
+      </c>
+      <c r="J56" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K56" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L56" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="M56" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N56" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O56" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P56" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q56" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D57" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E57" s="4">
+        <f>0.25*G57</f>
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="F57" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="G57" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="H57" s="2">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="I57" s="2">
+        <v>0</v>
+      </c>
+      <c r="J57" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K57" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L57" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="M57" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N57" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O57" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P57" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q57" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D58" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E58" s="4">
+        <f>0.3*G58</f>
+        <v>2.7E-2</v>
+      </c>
+      <c r="F58" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="G58" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="H58" s="2">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="I58" s="2">
+        <v>0</v>
+      </c>
+      <c r="J58" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K58" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L58" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="M58" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N58" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O58" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P58" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q58" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D59" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E59" s="4">
+        <f>0.35*G59</f>
+        <v>3.15E-2</v>
+      </c>
+      <c r="F59" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="G59" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="H59" s="2">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="I59" s="2">
+        <v>0</v>
+      </c>
+      <c r="J59" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K59" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L59" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="M59" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N59" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O59" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P59" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q59" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A60" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D60" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E60" s="4">
+        <f>0.4*G60</f>
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="F60" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="G60" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="H60" s="2">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="I60" s="2">
+        <v>0</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K60" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L60" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="M60" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N60" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O60" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P60" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q60" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A61" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D61" s="2">
+        <v>999999</v>
+      </c>
+      <c r="E61" s="4">
+        <f>0.45*G61</f>
+        <v>4.0500000000000001E-2</v>
+      </c>
+      <c r="F61" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="G61" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="H61" s="2">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="I61" s="2">
+        <v>0</v>
+      </c>
+      <c r="J61" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K61" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L61" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="M61" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N61" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O61" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P61" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q61" s="2" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on parameterization of GTR+GAMMA
</commit_message>
<xml_diff>
--- a/simulations_metadata.xlsx
+++ b/simulations_metadata.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28410"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -724,7 +724,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>